<commit_message>
Updated KVLCC2 geometry and HydRA run
</commit_message>
<xml_diff>
--- a/ros2_ws/src/mav_simulator/mav_simulator/hullform/KVLCC2/KVLCC2_Rudder.xlsx
+++ b/ros2_ws/src/mav_simulator/mav_simulator/hullform/KVLCC2/KVLCC2_Rudder.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Academics\Research\Github\makara\ros2_ws\src\mav_simulator\mav_simulator\hullform\KVLCC2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90346972-D8AF-4CC4-93BE-7DD8E30B0A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0CBB61-985A-4142-8ACA-AEC80696EB24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>Port</t>
   </si>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>Rudder height in prop slipstream (as per D) - Rhino</t>
-  </si>
-  <si>
-    <t>Rudder height in prop slipstream (as per Dp) - Rhino</t>
   </si>
   <si>
     <t>xp_R</t>
@@ -168,11 +165,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:I25"/>
+  <dimension ref="A2:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,14 +568,14 @@
       </c>
       <c r="F9">
         <f>SQRT((SQRT(1+8*B17/PI())+1) / (2 * (1 + B20*(SQRT(1 + 8*B17/PI())-1)))) * B9</f>
-        <v>7.5925399545568677</v>
+        <v>7.4155455986191479</v>
       </c>
       <c r="G9" t="s">
         <v>22</v>
       </c>
       <c r="H9">
         <f>F9/2</f>
-        <v>3.7962699772784338</v>
+        <v>3.7077727993095739</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -600,11 +598,11 @@
         <v>3.9027230589903067E-2</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12">
-        <f>(-148/B2+B3/2)/B3</f>
-        <v>3.7499999999999999E-2</v>
+        <v>26</v>
+      </c>
+      <c r="F12" s="2">
+        <f>B19/B3</f>
+        <v>2.0624999999999998E-2</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -616,9 +614,9 @@
         <v>0.63698910902512085</v>
       </c>
       <c r="E13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13">
+        <v>27</v>
+      </c>
+      <c r="F13" s="2">
         <v>-0.75</v>
       </c>
     </row>
@@ -631,17 +629,17 @@
         <v>0.62533282973403137</v>
       </c>
       <c r="E14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14">
+        <v>28</v>
+      </c>
+      <c r="F14" s="2">
         <v>0.6</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15">
+        <v>29</v>
+      </c>
+      <c r="F15" s="2">
         <v>0.3</v>
       </c>
     </row>
@@ -650,9 +648,10 @@
         <v>17</v>
       </c>
       <c r="B16">
-        <f>(B13+B14)/2</f>
-        <v>0.63116096937957611</v>
-      </c>
+        <f>B14</f>
+        <v>0.62533282973403137</v>
+      </c>
+      <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -660,21 +659,21 @@
       </c>
       <c r="B17">
         <f>B16/B12/B12</f>
-        <v>414.38561004015907</v>
+        <v>410.55917380663806</v>
       </c>
       <c r="E17" t="s">
-        <v>31</v>
-      </c>
-      <c r="F17">
+        <v>30</v>
+      </c>
+      <c r="F17" s="2">
         <f>1-0.75</f>
         <v>0.25</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18">
+        <v>31</v>
+      </c>
+      <c r="F18" s="2">
         <v>0</v>
       </c>
     </row>
@@ -683,19 +682,18 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <f>4/B2</f>
-        <v>4</v>
+        <v>6.6</v>
       </c>
       <c r="C19">
         <f>B19/B9</f>
-        <v>0.40567951318458423</v>
+        <v>0.66937119675456391</v>
       </c>
       <c r="E19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19">
+        <v>32</v>
+      </c>
+      <c r="F19" s="2">
         <f>F12</f>
-        <v>3.7499999999999999E-2</v>
+        <v>2.0624999999999998E-2</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -704,20 +702,20 @@
       </c>
       <c r="B20">
         <f>0.5 + 0.5*(B19/B9) / ((B19/B9) + 0.15)</f>
-        <v>0.86503011498448623</v>
-      </c>
+        <v>0.90846639435573706</v>
+      </c>
+      <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21">
+        <v>33</v>
+      </c>
+      <c r="F21" s="2">
         <f>G21/B3/B3</f>
-        <v>5.5935546875000007E-4</v>
+        <v>2.6689453125000001E-3</v>
       </c>
       <c r="G21">
-        <f>57.278/B2/B2</f>
-        <v>57.277999999999999</v>
+        <v>273.3</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -725,39 +723,33 @@
         <v>23</v>
       </c>
       <c r="B22">
-        <v>5</v>
-      </c>
+        <v>15.8</v>
+      </c>
+      <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23">
-        <v>4</v>
+        <f>F9</f>
+        <v>7.4155455986191479</v>
       </c>
       <c r="E23" t="s">
-        <v>35</v>
-      </c>
-      <c r="F23">
+        <v>34</v>
+      </c>
+      <c r="F23" s="2">
         <f>5/4</f>
         <v>1.25</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>25</v>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>24</v>
       </c>
       <c r="B24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25">
-        <f>B24/B22</f>
-        <v>0.6</v>
+        <f>B23/B22</f>
+        <v>0.46933832902652833</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated aspect ratio of rudder in excel file
</commit_message>
<xml_diff>
--- a/ros2_ws/src/mav_simulator/mav_simulator/hullform/KVLCC2/KVLCC2_Rudder.xlsx
+++ b/ros2_ws/src/mav_simulator/mav_simulator/hullform/KVLCC2/KVLCC2_Rudder.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Academics\Research\Github\makara\ros2_ws\src\mav_simulator\mav_simulator\hullform\KVLCC2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Academics\Research\makara\ros2_ws\src\mav_simulator\mav_simulator\hullform\KVLCC2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0CBB61-985A-4142-8ACA-AEC80696EB24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CCEAF0-79B5-4855-99FD-CA3DD73E7E8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,15 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -165,12 +174,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,17 +462,17 @@
   <dimension ref="A2:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -478,7 +486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -498,7 +506,7 @@
         <v>-8.5785749999999994E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -518,7 +526,7 @@
         <v>-0.29107261000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -538,7 +546,7 @@
         <v>0.63682324999999995</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -547,7 +555,7 @@
         <v>7.9546975424587947</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -556,7 +564,7 @@
         <v>13.333333333333334</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -578,7 +586,7 @@
         <v>3.7077727993095739</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -589,7 +597,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -600,12 +608,12 @@
       <c r="E12" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12">
         <f>B19/B3</f>
         <v>2.0624999999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -616,11 +624,11 @@
       <c r="E13" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13">
         <v>-0.75</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -631,19 +639,19 @@
       <c r="E14" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14">
         <v>0.6</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="E15" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15">
         <v>0.3</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -651,9 +659,8 @@
         <f>B14</f>
         <v>0.62533282973403137</v>
       </c>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -664,20 +671,20 @@
       <c r="E17" t="s">
         <v>30</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17">
         <f>1-0.75</f>
         <v>0.25</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E18" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -691,12 +698,12 @@
       <c r="E19" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19">
         <f>F12</f>
         <v>2.0624999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -704,13 +711,12 @@
         <f>0.5 + 0.5*(B19/B9) / ((B19/B9) + 0.15)</f>
         <v>0.90846639435573706</v>
       </c>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E21" t="s">
         <v>33</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21">
         <f>G21/B3/B3</f>
         <v>2.6689453125000001E-3</v>
       </c>
@@ -718,16 +724,15 @@
         <v>273.3</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>23</v>
       </c>
       <c r="B22">
         <v>15.8</v>
       </c>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -738,12 +743,12 @@
       <c r="E23" t="s">
         <v>34</v>
       </c>
-      <c r="F23" s="2">
-        <f>5/4</f>
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <f>B22/(3.5+5.14)</f>
+        <v>1.8287037037037037</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>24</v>
       </c>

</xml_diff>